<commit_message>
Create api quote fee
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/Booking_Quote_Fee.xlsx
+++ b/src/main/resources/input_excel_file/Booking_Quote_Fee.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>tc_id</t>
   </si>
@@ -39,85 +39,251 @@
     <t>expected_result</t>
   </si>
   <si>
-    <t>course_uid</t>
-  </si>
-  <si>
-    <t>partner_uid</t>
+    <t>booking_date</t>
+  </si>
+  <si>
+    <t>agency_id</t>
   </si>
   <si>
     <t>list_player</t>
   </si>
   <si>
-    <t>agency_id</t>
-  </si>
-  <si>
-    <t>booking_date</t>
-  </si>
-  <si>
     <t>expected_validation_data</t>
   </si>
   <si>
-    <t>TC_0001</t>
-  </si>
-  <si>
-    <t>Verify Login Success</t>
+    <t>QF_001</t>
+  </si>
+  <si>
+    <t>Verify quote fee for 2 player successfully</t>
   </si>
   <si>
     <t>success</t>
   </si>
   <si>
-    <t>CHI-LINH</t>
-  </si>
-  <si>
-    <t>CHI-LINH-01</t>
-  </si>
-  <si>
-    <t>[
+    <t xml:space="preserve"> [
         {
-            "booking_date": "{{current_booking_date}}",
-            "guest_style": "5D_package_PTT",
+            "booking_date": "10/08/2025",
+            "guest_style": "5D_PTT",
             "caddie_code": "",
             "tee_type": "1",
-            "tee_time": "20:58",
+            "tee_time": "18:00",
             "hole": 18,
             "add_ons": [],
-            "player_idx": "13:0810",
+            "player_idx": "18:0010",
+            "voucher_apply": []
+        },
+        {
+            "booking_date": "10/08/2025",
+            "guest_style": "5D_PTT",
+            "caddie_code": "",
+            "tee_type": "1",
+            "tee_time": "18:00",
+            "hole": 18,
+            "add_ons": [],
+            "player_idx": "18:0011",
             "voucher_apply": []
         }
     ]</t>
   </si>
   <si>
-    <t>{{Date}}</t>
-  </si>
-  <si>
-    <t>{"token": "NOT_NULL", "data.user_name": "phuongtt-chilinh"}</t>
-  </si>
-  <si>
-    <t>TC_0002</t>
-  </si>
-  <si>
-    <t>Verify Login Wrong Username</t>
+    <t>{
+    "status_code": 200,
+    "total_amount": 3000000,
+    "list_player.size()": 2,
+    "list_player[0].total_fee": 1500000,
+    "list_player[0].player_idx": "18:0010",
+    "list_player[1].total_fee": 1500000,
+    "list_player[1].player_idx": "18:0011"
+}</t>
+  </si>
+  <si>
+    <t>QF_002</t>
+  </si>
+  <si>
+    <t>Verify quote fee for 1 player successfully</t>
+  </si>
+  <si>
+    <t>{{TODAY}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [
+        {
+            "booking_date": "10/08/2025",
+            "guest_style": "5D_PTT",
+            "caddie_code": "",
+            "tee_type": "1",
+            "tee_time": "18:00",
+            "hole": 18,
+            "add_ons": [],
+            "player_idx": "18:0010",
+            "voucher_apply": []
+        }
+    ]</t>
+  </si>
+  <si>
+    <t>{"status_code": 200, "list_player.size()": 1, "total_amount": "NOT_NULL"}</t>
+  </si>
+  <si>
+    <t>QF_003</t>
+  </si>
+  <si>
+    <t>Verify quote fee for 4 players successfully</t>
+  </si>
+  <si>
+    <t>{{TODAY+7}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [
+        {
+            "booking_date": "{{TODAY+7}}",
+            "guest_style": "5D_PTT",
+            "caddie_code": "",
+            "tee_type": "1",
+            "tee_time": "18:00",
+            "hole": 18,
+            "add_ons": [],
+            "player_idx": "18:0010",
+            "voucher_apply": []
+        },
+        {
+            "booking_date": "{{TODAY+7}}",
+            "guest_style": "5D_PTT",
+            "caddie_code": "",
+            "tee_type": "1",
+            "tee_time": "18:00",
+            "hole": 18,
+            "add_ons": [],
+            "player_idx": "18:0011",
+            "voucher_apply": []
+        },
+        {
+            "booking_date": "{{TODAY+7}}",
+            "guest_style": "5D_PTT",
+            "caddie_code": "",
+            "tee_type": "1",
+            "tee_time": "18:00",
+            "hole": 18,
+            "add_ons": [],
+            "player_idx": "18:0012",
+            "voucher_apply": []
+        },
+        {
+            "booking_date": "{{TODAY+7}}",
+            "guest_style": "5D_PTT",
+            "caddie_code": "",
+            "tee_type": "1",
+            "tee_time": "18:00",
+            "hole": 18,
+            "add_ons": [],
+            "player_idx": "18:0013",
+            "voucher_apply": []
+        }
+    ]</t>
+  </si>
+  <si>
+    <t>{"status_code": 200, "list_player.size()": 4, "total_amount": "NOT_NULL"}</t>
+  </si>
+  <si>
+    <t>QF_004</t>
+  </si>
+  <si>
+    <t>Verify error when player list is empty</t>
   </si>
   <si>
     <t>failed</t>
   </si>
   <si>
-    <t>{"status_code": 500}</t>
-  </si>
-  <si>
-    <t>TC_0003</t>
-  </si>
-  <si>
-    <t>Verify Login Wrong Password</t>
+    <t>[]</t>
   </si>
   <si>
     <t>{"status_code": 400}</t>
   </si>
   <si>
-    <t>TC_0004</t>
-  </si>
-  <si>
-    <t>Verify Login Wrong Username And Password</t>
+    <t>QF_005</t>
+  </si>
+  <si>
+    <t>Verify error when guest_style is missing</t>
+  </si>
+  <si>
+    <t>[{"booking_date": "{{TODAY}}", "tee_type": "1", "tee_time": "10:00", "hole": 18}]</t>
+  </si>
+  <si>
+    <t>{"status_code": 400, "key": "GUEST_STYLE_IS_REQUIRED"}</t>
+  </si>
+  <si>
+    <t>QF_006</t>
+  </si>
+  <si>
+    <t>Verify error when agency_id is a string</t>
+  </si>
+  <si>
+    <t>WRONG_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [
+        {
+            "booking_date": "{{TODAY}}",
+            "guest_style": "5D_PTT",
+            "caddie_code": "",
+            "tee_type": "1",
+            "tee_time": "18:00",
+            "hole": 18,
+            "add_ons": [],
+            "player_idx": "18:0010",
+            "voucher_apply": []
+        }
+    ]</t>
+  </si>
+  <si>
+    <t>QF_007</t>
+  </si>
+  <si>
+    <t>Verify error when booking date is in the past</t>
+  </si>
+  <si>
+    <t>{{TODAY-1}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [
+        {
+            "booking_date": "{{TODAY-1}}",
+            "guest_style": "5D_PTT",
+            "caddie_code": "",
+            "tee_type": "1",
+            "tee_time": "18:00",
+            "hole": 18,
+            "add_ons": [],
+            "player_idx": "18:0010",
+            "voucher_apply": []
+        }
+    ]</t>
+  </si>
+  <si>
+    <t>{"status_code": 400, "key": "INVALID_BOOKING_DATE"}</t>
+  </si>
+  <si>
+    <t>QF_008</t>
+  </si>
+  <si>
+    <t>Verify error when guest_style is invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [
+        {
+            "booking_date": "{{TODAY}}",
+            "guest_style": "INVALID_GUEST_STYLE",
+            "caddie_code": "",
+            "tee_type": "1",
+            "tee_time": "18:00",
+            "hole": 18,
+            "add_ons": [],
+            "player_idx": "18:0010",
+            "voucher_apply": []
+        }
+    ]</t>
+  </si>
+  <si>
+    <t>{"status_code": 400, "key": "INVALID_GUEST_STYLE"}</t>
   </si>
   <si>
     <t>endpoint</t>
@@ -149,12 +315,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +348,42 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF1A1C1E"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF1A1C1E"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -326,7 +528,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +549,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFCFCFC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -526,7 +734,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -596,17 +804,28 @@
     </border>
     <border>
       <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -619,8 +838,34 @@
       <top style="medium">
         <color rgb="FFCCCCCC"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -730,149 +975,149 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -891,14 +1136,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1433,136 +1705,227 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="21.8571428571429" customWidth="1"/>
-    <col min="4" max="5" width="18.8571428571429" customWidth="1"/>
-    <col min="6" max="6" width="55.8571428571429" customWidth="1"/>
-    <col min="7" max="7" width="18.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="19.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="37.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="9.14285714285714" style="6"/>
+    <col min="2" max="2" width="30" style="6" customWidth="1"/>
+    <col min="3" max="5" width="21.8571428571429" style="6" customWidth="1"/>
+    <col min="6" max="6" width="55.8571428571429" style="6" customWidth="1"/>
+    <col min="7" max="7" width="40.1238095238095" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="9.14285714285714" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="27" customHeight="1" spans="1:7">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+    </row>
+    <row r="2" ht="378" spans="1:7">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="14">
+        <v>45879</v>
+      </c>
+      <c r="E2" s="13">
+        <v>95</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" ht="205.5" spans="1:9">
-      <c r="A2" s="3" t="s">
+    <row r="3" ht="173" customHeight="1" spans="1:7">
+      <c r="A3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="D3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4">
+      <c r="E3" s="17">
         <v>95</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="F3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="G3" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" ht="29" customHeight="1" spans="1:9">
-      <c r="A3" s="3" t="s">
+    <row r="4" ht="82" customHeight="1" spans="1:7">
+      <c r="A4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
+      <c r="E4" s="17">
+        <v>95</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>20</v>
       </c>
+      <c r="G4" s="16" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" ht="16.5" spans="1:9">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="5" ht="51" customHeight="1" spans="1:7">
+      <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>23</v>
       </c>
+      <c r="C5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="17">
+        <v>95</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" ht="35" customHeight="1" spans="1:9">
-      <c r="A5" s="3" t="s">
+    <row r="6" ht="59" customHeight="1" spans="1:7">
+      <c r="A6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
-        <v>20</v>
+      <c r="D6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="17">
+        <v>95</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" ht="165.75" spans="1:7">
+      <c r="A7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" ht="165.75" spans="1:7">
+      <c r="A8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="17">
+        <v>95</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" ht="165.75" spans="1:7">
+      <c r="A9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="17">
+        <v>95</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1582,7 +1945,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="31.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="41.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="16.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="38.5714285714286" customWidth="1"/>
     <col min="4" max="4" width="31.2857142857143" customWidth="1"/>
@@ -1590,30 +1953,30 @@
   <sheetData>
     <row r="1" ht="19.5" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" ht="24" customHeight="1" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>